<commit_message>
3.12-3.18 + fixed a bug in id assignation in front end
</commit_message>
<xml_diff>
--- a/fullstackopen.xlsx
+++ b/fullstackopen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olenj\Desktop\Reactihommia\Full Stack Open\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF337D33-42BA-45A5-9D05-2D855D4EE68B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817E7F9D-4AEC-4EA7-B72A-46C87A9AD0E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A39D8CF8-623D-4699-BD5A-AA6F35350729}"/>
   </bookViews>
@@ -974,10 +974,10 @@
     <t>Yhteensä: 297</t>
   </si>
   <si>
-    <t>Tehty: 36</t>
-  </si>
-  <si>
     <t>Maali 7op arvosana 5</t>
+  </si>
+  <si>
+    <t>Tehty: 54</t>
   </si>
 </sst>
 </file>
@@ -1647,7 +1647,7 @@
   <dimension ref="B3:AC28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,34 +1923,34 @@
       <c r="J11" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="K11" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="L11" s="20" t="s">
+      <c r="L11" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="M11" s="20" t="s">
+      <c r="M11" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="N11" s="20" t="s">
+      <c r="N11" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="O11" s="20" t="s">
+      <c r="O11" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="P11" s="20" t="s">
+      <c r="P11" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="Q11" s="20" t="s">
+      <c r="Q11" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="R11" s="20" t="s">
+      <c r="R11" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S11" s="20" t="s">
+      <c r="S11" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="T11" s="20" t="s">
+      <c r="T11" s="19" t="s">
         <v>63</v>
       </c>
       <c r="U11" s="20" t="s">
@@ -2764,24 +2764,24 @@
     </row>
     <row r="24" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B24" s="24" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="25" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B25">
-        <f>36/116</f>
-        <v>0.31034482758620691</v>
+        <f>54/116</f>
+        <v>0.46551724137931033</v>
       </c>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B26">
-        <f>36/138</f>
-        <v>0.2608695652173913</v>
+        <f>54/138</f>
+        <v>0.39130434782608697</v>
       </c>
     </row>
     <row r="28" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B28" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4.6 & 4.7 done
</commit_message>
<xml_diff>
--- a/fullstackopen.xlsx
+++ b/fullstackopen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olenj\Desktop\Reactihommia\Full Stack Open\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B754B87D-4EE5-4D51-90E4-56E7769215DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C456D6-7719-4252-A411-5C5F21DF167C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A39D8CF8-623D-4699-BD5A-AA6F35350729}"/>
   </bookViews>
@@ -965,9 +965,6 @@
     <t>13.24</t>
   </si>
   <si>
-    <t>Yhteensä: 297</t>
-  </si>
-  <si>
     <t>Maali 7op arvosana 5</t>
   </si>
   <si>
@@ -980,7 +977,10 @@
     <t>5op 1/5</t>
   </si>
   <si>
-    <t>Tehty: 63</t>
+    <t xml:space="preserve">Tehty: </t>
+  </si>
+  <si>
+    <t>Yhteensä:</t>
   </si>
 </sst>
 </file>
@@ -1241,7 +1241,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1299,9 +1299,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
@@ -1315,8 +1312,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFEB9C"/>
       <color rgb="FFC6EFCE"/>
-      <color rgb="FFFFEB9C"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1650,7 +1647,7 @@
   <dimension ref="B3:AC28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1986,7 +1983,7 @@
       <c r="F12" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="19" t="s">
         <v>71</v>
       </c>
       <c r="H12" s="20" t="s">
@@ -2225,7 +2222,7 @@
       <c r="G15" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="H15" s="20" t="s">
         <v>145</v>
       </c>
       <c r="I15" s="20" t="s">
@@ -2758,21 +2755,27 @@
     </row>
     <row r="23" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B23" s="24" t="s">
-        <v>309</v>
+        <v>314</v>
+      </c>
+      <c r="C23">
+        <v>295</v>
       </c>
     </row>
     <row r="24" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B24" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
+      </c>
+      <c r="C24">
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B25">
-        <f>63/116</f>
-        <v>0.5431034482758621</v>
+        <f>C24/116</f>
+        <v>0.55172413793103448</v>
       </c>
       <c r="C25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K25">
         <f>63/295</f>
@@ -2781,25 +2784,25 @@
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B26">
-        <f>63/138</f>
-        <v>0.45652173913043476</v>
+        <f>C24/138</f>
+        <v>0.46376811594202899</v>
       </c>
       <c r="C26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B27">
-        <f>63/72</f>
-        <v>0.875</v>
+        <f>C24/72</f>
+        <v>0.88888888888888884</v>
       </c>
       <c r="C27" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B28" s="26" t="s">
-        <v>310</v>
+      <c r="B28" s="25" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Valmistelut 4.8:lle, testejä aloitettu, eri databasen käyttö testejä ajaessa.
</commit_message>
<xml_diff>
--- a/fullstackopen.xlsx
+++ b/fullstackopen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olenj\Desktop\Reactihommia\Full Stack Open\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C456D6-7719-4252-A411-5C5F21DF167C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB236F6-F447-4EBD-B055-EB24D13F4635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A39D8CF8-623D-4699-BD5A-AA6F35350729}"/>
   </bookViews>
@@ -1312,8 +1312,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFC6EFCE"/>
       <color rgb="FFFFEB9C"/>
-      <color rgb="FFC6EFCE"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1647,7 +1647,7 @@
   <dimension ref="B3:AC28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+      <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1986,10 +1986,10 @@
       <c r="G12" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="19" t="s">
         <v>73</v>
       </c>
       <c r="J12" s="20" t="s">
@@ -2766,13 +2766,13 @@
         <v>313</v>
       </c>
       <c r="C24">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B25">
         <f>C24/116</f>
-        <v>0.55172413793103448</v>
+        <v>0.56896551724137934</v>
       </c>
       <c r="C25" t="s">
         <v>311</v>
@@ -2785,7 +2785,7 @@
     <row r="26" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B26">
         <f>C24/138</f>
-        <v>0.46376811594202899</v>
+        <v>0.47826086956521741</v>
       </c>
       <c r="C26" t="s">
         <v>310</v>
@@ -2794,7 +2794,7 @@
     <row r="27" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B27">
         <f>C24/72</f>
-        <v>0.88888888888888884</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="C27" t="s">
         <v>312</v>

</xml_diff>